<commit_message>
tidy water sample data
</commit_message>
<xml_diff>
--- a/data/raw/2024-02-28_water-samples.xlsx
+++ b/data/raw/2024-02-28_water-samples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lysbethkoster/Documents/Universiteit/University of Hawai'i/MSc Thesis/Thesis/RQ2/nomilo-fishpond-analysis/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7679F0AA-2D11-364C-8E0D-EAC35A1C1058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6285CBA7-10C2-2349-B276-B15624E1557C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="160">
   <si>
     <t>S-LAB Value</t>
     <phoneticPr fontId="7" type="noConversion"/>
@@ -404,24 +404,6 @@
   </si>
   <si>
     <t>20/02/2024</t>
-  </si>
-  <si>
-    <t>Location ID</t>
-  </si>
-  <si>
-    <t>Back Buoy</t>
-  </si>
-  <si>
-    <t>Mid Buoy</t>
-  </si>
-  <si>
-    <t>Production Dock</t>
-  </si>
-  <si>
-    <t>Auwei</t>
-  </si>
-  <si>
-    <t>Well</t>
   </si>
   <si>
     <t>Depth (m)</t>
@@ -690,12 +672,12 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -735,12 +717,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,7 +1034,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1196,6 +1172,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1232,22 +1218,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1709,7 +1684,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1731,22 +1706,22 @@
   <sheetData>
     <row r="1" spans="1:18" s="55" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C1" s="70" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D1" s="55" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="90" t="s">
+      <c r="E1" s="55" t="s">
         <v>99</v>
       </c>
       <c r="F1" s="55" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G1" s="55" t="s">
         <v>101</v>
@@ -1758,31 +1733,31 @@
         <v>103</v>
       </c>
       <c r="J1" s="55" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="K1" s="55" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="71" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="N1" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="O1" s="71" t="s">
+        <v>117</v>
+      </c>
+      <c r="P1" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q1" s="71" t="s">
+        <v>119</v>
+      </c>
+      <c r="R1" s="71" t="s">
         <v>120</v>
-      </c>
-      <c r="M1" s="84" t="s">
-        <v>121</v>
-      </c>
-      <c r="N1" s="83" t="s">
-        <v>122</v>
-      </c>
-      <c r="O1" s="83" t="s">
-        <v>123</v>
-      </c>
-      <c r="P1" s="83" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q1" s="83" t="s">
-        <v>125</v>
-      </c>
-      <c r="R1" s="83" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.15">
@@ -1796,7 +1771,7 @@
         <v>105</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F2">
         <v>4</v>
@@ -1816,26 +1791,26 @@
       <c r="K2" s="65">
         <v>0.55166376981550902</v>
       </c>
-      <c r="L2" s="86">
+      <c r="L2" s="73">
         <v>6759866.666666667</v>
       </c>
-      <c r="M2" s="86">
+      <c r="M2" s="73">
         <v>45316.666666666672</v>
       </c>
-      <c r="N2" s="86">
+      <c r="N2" s="73">
         <v>1832883.3333333335</v>
       </c>
-      <c r="O2" s="86">
+      <c r="O2" s="73">
         <v>82200</v>
       </c>
-      <c r="P2" s="86">
+      <c r="P2" s="73">
         <v>73166.666666666672</v>
       </c>
-      <c r="Q2" s="86">
+      <c r="Q2" s="73">
         <v>16700</v>
       </c>
-      <c r="R2" s="88" t="s">
-        <v>127</v>
+      <c r="R2" s="74" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
@@ -1849,7 +1824,7 @@
         <v>105</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F3">
         <v>0.5</v>
@@ -1869,26 +1844,26 @@
       <c r="K3" s="65">
         <v>7.5972190228886141E-2</v>
       </c>
-      <c r="L3" s="86">
+      <c r="L3" s="73">
         <v>6491183.333333334</v>
       </c>
-      <c r="M3" s="86">
+      <c r="M3" s="73">
         <v>34983.333333333336</v>
       </c>
-      <c r="N3" s="86">
+      <c r="N3" s="73">
         <v>1684616.6666666667</v>
       </c>
-      <c r="O3" s="86">
+      <c r="O3" s="73">
         <v>72350</v>
       </c>
-      <c r="P3" s="86">
+      <c r="P3" s="73">
         <v>54250</v>
       </c>
-      <c r="Q3" s="86">
+      <c r="Q3" s="73">
         <v>13266.666666666668</v>
       </c>
-      <c r="R3" s="88" t="s">
-        <v>128</v>
+      <c r="R3" s="74" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -1902,7 +1877,7 @@
         <v>105</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F4">
         <v>7.5</v>
@@ -1922,26 +1897,26 @@
       <c r="K4" s="65">
         <v>3.2685653257386971</v>
       </c>
-      <c r="L4" s="86">
+      <c r="L4" s="73">
         <v>7585816.666666667</v>
       </c>
-      <c r="M4" s="86">
+      <c r="M4" s="73">
         <v>78016.666666666672</v>
       </c>
-      <c r="N4" s="86">
+      <c r="N4" s="73">
         <v>1846716.6666666667</v>
       </c>
-      <c r="O4" s="86">
+      <c r="O4" s="73">
         <v>235600</v>
       </c>
-      <c r="P4" s="86">
+      <c r="P4" s="73">
         <v>197316.66666666669</v>
       </c>
-      <c r="Q4" s="86">
+      <c r="Q4" s="73">
         <v>17050</v>
       </c>
-      <c r="R4" s="88" t="s">
-        <v>129</v>
+      <c r="R4" s="74" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
@@ -1955,7 +1930,7 @@
         <v>105</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F5">
         <v>4</v>
@@ -1975,26 +1950,26 @@
       <c r="K5" s="65">
         <v>1.0934286851087889</v>
       </c>
-      <c r="L5" s="86">
+      <c r="L5" s="73">
         <v>6778516.666666667</v>
       </c>
-      <c r="M5" s="86">
+      <c r="M5" s="73">
         <v>32400</v>
       </c>
-      <c r="N5" s="86">
+      <c r="N5" s="73">
         <v>1813683.3333333335</v>
       </c>
-      <c r="O5" s="86">
+      <c r="O5" s="73">
         <v>78166.666666666672</v>
       </c>
-      <c r="P5" s="86">
+      <c r="P5" s="73">
         <v>63916.666666666672</v>
       </c>
-      <c r="Q5" s="86">
+      <c r="Q5" s="73">
         <v>17400</v>
       </c>
-      <c r="R5" s="88" t="s">
-        <v>130</v>
+      <c r="R5" s="74" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
@@ -2008,7 +1983,7 @@
         <v>105</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F6">
         <v>0.5</v>
@@ -2028,26 +2003,26 @@
       <c r="K6" s="65">
         <v>0.11344208740812095</v>
       </c>
-      <c r="L6" s="86">
+      <c r="L6" s="73">
         <v>6064683.333333334</v>
       </c>
-      <c r="M6" s="86">
+      <c r="M6" s="73">
         <v>29983.333333333336</v>
       </c>
-      <c r="N6" s="86">
+      <c r="N6" s="73">
         <v>1564583.3333333335</v>
       </c>
-      <c r="O6" s="86">
+      <c r="O6" s="73">
         <v>66050</v>
       </c>
-      <c r="P6" s="86">
+      <c r="P6" s="73">
         <v>46066.666666666672</v>
       </c>
-      <c r="Q6" s="86">
+      <c r="Q6" s="73">
         <v>13716.666666666668</v>
       </c>
-      <c r="R6" s="88" t="s">
-        <v>131</v>
+      <c r="R6" s="74" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
@@ -2061,7 +2036,7 @@
         <v>105</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F7">
         <v>2.75</v>
@@ -2081,26 +2056,26 @@
       <c r="K7" s="65">
         <v>0.32313990744037024</v>
       </c>
-      <c r="L7" s="86">
+      <c r="L7" s="73">
         <v>5856783.333333334</v>
       </c>
-      <c r="M7" s="86">
+      <c r="M7" s="73">
         <v>28450</v>
       </c>
-      <c r="N7" s="86">
+      <c r="N7" s="73">
         <v>1384566.6666666667</v>
       </c>
-      <c r="O7" s="86">
+      <c r="O7" s="73">
         <v>60383.333333333336</v>
       </c>
-      <c r="P7" s="86">
+      <c r="P7" s="73">
         <v>45783.333333333336</v>
       </c>
-      <c r="Q7" s="86">
+      <c r="Q7" s="73">
         <v>11733.333333333334</v>
       </c>
-      <c r="R7" s="88" t="s">
-        <v>132</v>
+      <c r="R7" s="74" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
@@ -2114,7 +2089,7 @@
         <v>105</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F8">
         <v>0.5</v>
@@ -2134,26 +2109,26 @@
       <c r="K8" s="65">
         <v>0.47799928800284797</v>
       </c>
-      <c r="L8" s="86">
+      <c r="L8" s="73">
         <v>5806383.333333334</v>
       </c>
-      <c r="M8" s="86">
+      <c r="M8" s="73">
         <v>20600</v>
       </c>
-      <c r="N8" s="86">
+      <c r="N8" s="73">
         <v>1467483.3333333335</v>
       </c>
-      <c r="O8" s="86">
+      <c r="O8" s="73">
         <v>63850</v>
       </c>
-      <c r="P8" s="86">
+      <c r="P8" s="73">
         <v>38333.333333333336</v>
       </c>
-      <c r="Q8" s="86">
+      <c r="Q8" s="73">
         <v>8516.6666666666679</v>
       </c>
-      <c r="R8" s="88" t="s">
-        <v>133</v>
+      <c r="R8" s="74" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.2">
@@ -2167,7 +2142,7 @@
         <v>105</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F9">
         <v>0.5</v>
@@ -2184,26 +2159,26 @@
       <c r="K9" s="65">
         <v>10.237966201076372</v>
       </c>
-      <c r="L9" s="87">
+      <c r="L9" s="88">
         <v>1522316.6666666667</v>
       </c>
-      <c r="M9" s="87">
+      <c r="M9" s="88">
         <v>403766.66666666669</v>
       </c>
-      <c r="N9" s="87">
+      <c r="N9" s="88">
         <v>65216.666666666672</v>
       </c>
-      <c r="O9" s="87">
+      <c r="O9" s="88">
         <v>6916.666666666667</v>
       </c>
-      <c r="P9" s="87">
+      <c r="P9" s="88">
         <v>93783.333333333343</v>
       </c>
-      <c r="Q9" s="87">
+      <c r="Q9" s="88">
         <v>616.66666666666674</v>
       </c>
       <c r="R9" s="89" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
@@ -2217,7 +2192,7 @@
         <v>105</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F10">
         <v>0.75</v>
@@ -2237,26 +2212,26 @@
       <c r="K10" s="65">
         <v>0.29314368064819812</v>
       </c>
-      <c r="L10" s="86">
+      <c r="L10" s="73">
         <v>5276316.666666667</v>
       </c>
-      <c r="M10" s="86">
+      <c r="M10" s="73">
         <v>28016.666666666668</v>
       </c>
-      <c r="N10" s="86">
+      <c r="N10" s="73">
         <v>1310716.6666666667</v>
       </c>
-      <c r="O10" s="86">
+      <c r="O10" s="73">
         <v>54166.666666666672</v>
       </c>
-      <c r="P10" s="86">
+      <c r="P10" s="73">
         <v>40900</v>
       </c>
-      <c r="Q10" s="86">
+      <c r="Q10" s="73">
         <v>11283.333333333334</v>
       </c>
-      <c r="R10" s="88" t="s">
-        <v>135</v>
+      <c r="R10" s="74" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
@@ -2270,7 +2245,7 @@
         <v>105</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F11">
         <v>0.5</v>
@@ -2287,26 +2262,26 @@
       <c r="K11" s="65">
         <v>1.1989759805666658</v>
       </c>
-      <c r="L11" s="86">
+      <c r="L11" s="73">
         <v>1542116.6666666667</v>
       </c>
-      <c r="M11" s="86">
+      <c r="M11" s="73">
         <v>11400</v>
       </c>
-      <c r="N11" s="86">
+      <c r="N11" s="73">
         <v>330783.33333333337</v>
       </c>
-      <c r="O11" s="86">
+      <c r="O11" s="73">
         <v>16583.333333333336</v>
       </c>
-      <c r="P11" s="86">
+      <c r="P11" s="73">
         <v>24150</v>
       </c>
-      <c r="Q11" s="86">
+      <c r="Q11" s="73">
         <v>2133.3333333333335</v>
       </c>
-      <c r="R11" s="88" t="s">
-        <v>136</v>
+      <c r="R11" s="74" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.15">
@@ -2320,7 +2295,7 @@
         <v>106</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F12">
         <v>4</v>
@@ -2340,13 +2315,13 @@
       <c r="K12" s="65">
         <v>0.17575021464620025</v>
       </c>
-      <c r="L12" s="85"/>
-      <c r="M12" s="85"/>
-      <c r="N12" s="85"/>
-      <c r="O12" s="85"/>
-      <c r="P12" s="85"/>
-      <c r="Q12" s="85"/>
-      <c r="R12" s="85"/>
+      <c r="L12" s="87"/>
+      <c r="M12" s="87"/>
+      <c r="N12" s="87"/>
+      <c r="O12" s="87"/>
+      <c r="P12" s="87"/>
+      <c r="Q12" s="87"/>
+      <c r="R12" s="87"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B13" s="68">
@@ -2359,7 +2334,7 @@
         <v>106</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F13">
         <v>0.5</v>
@@ -2379,13 +2354,13 @@
       <c r="K13" s="65">
         <v>0.50490230980252548</v>
       </c>
-      <c r="L13" s="85"/>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
-      <c r="R13" s="85"/>
+      <c r="L13" s="87"/>
+      <c r="M13" s="87"/>
+      <c r="N13" s="87"/>
+      <c r="O13" s="87"/>
+      <c r="P13" s="87"/>
+      <c r="Q13" s="87"/>
+      <c r="R13" s="87"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B14" s="68">
@@ -2398,7 +2373,7 @@
         <v>106</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F14">
         <v>7.5</v>
@@ -2418,13 +2393,13 @@
       <c r="K14" s="65">
         <v>5.717590517873222</v>
       </c>
-      <c r="L14" s="85"/>
-      <c r="M14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="87"/>
+      <c r="O14" s="87"/>
+      <c r="P14" s="87"/>
+      <c r="Q14" s="87"/>
+      <c r="R14" s="87"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B15" s="68">
@@ -2437,7 +2412,7 @@
         <v>106</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F15">
         <v>4</v>
@@ -2457,13 +2432,13 @@
       <c r="K15" s="65">
         <v>0.1225544217838834</v>
       </c>
-      <c r="L15" s="85"/>
-      <c r="M15" s="85"/>
-      <c r="N15" s="85"/>
-      <c r="O15" s="85"/>
-      <c r="P15" s="85"/>
-      <c r="Q15" s="85"/>
-      <c r="R15" s="85"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.15">
       <c r="B16" s="68">
@@ -2476,7 +2451,7 @@
         <v>106</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F16">
         <v>0.5</v>
@@ -2496,13 +2471,13 @@
       <c r="K16" s="65">
         <v>0.40063032689045719</v>
       </c>
-      <c r="L16" s="85"/>
-      <c r="M16" s="85"/>
-      <c r="N16" s="85"/>
-      <c r="O16" s="85"/>
-      <c r="P16" s="85"/>
-      <c r="Q16" s="85"/>
-      <c r="R16" s="85"/>
+      <c r="L16" s="87"/>
+      <c r="M16" s="87"/>
+      <c r="N16" s="87"/>
+      <c r="O16" s="87"/>
+      <c r="P16" s="87"/>
+      <c r="Q16" s="87"/>
+      <c r="R16" s="87"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B17" s="68">
@@ -2515,7 +2490,7 @@
         <v>106</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F17">
         <v>2.75</v>
@@ -2535,13 +2510,13 @@
       <c r="K17" s="65">
         <v>0.22172219546415931</v>
       </c>
-      <c r="L17" s="85"/>
-      <c r="M17" s="85"/>
-      <c r="N17" s="85"/>
-      <c r="O17" s="85"/>
-      <c r="P17" s="85"/>
-      <c r="Q17" s="85"/>
-      <c r="R17" s="85"/>
+      <c r="L17" s="87"/>
+      <c r="M17" s="87"/>
+      <c r="N17" s="87"/>
+      <c r="O17" s="87"/>
+      <c r="P17" s="87"/>
+      <c r="Q17" s="87"/>
+      <c r="R17" s="87"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B18" s="68">
@@ -2554,7 +2529,7 @@
         <v>106</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F18">
         <v>0.5</v>
@@ -2574,13 +2549,13 @@
       <c r="K18" s="65">
         <v>0.46476032919397736</v>
       </c>
-      <c r="L18" s="85"/>
-      <c r="M18" s="85"/>
-      <c r="N18" s="85"/>
-      <c r="O18" s="85"/>
-      <c r="P18" s="85"/>
-      <c r="Q18" s="85"/>
-      <c r="R18" s="85"/>
+      <c r="L18" s="87"/>
+      <c r="M18" s="87"/>
+      <c r="N18" s="87"/>
+      <c r="O18" s="87"/>
+      <c r="P18" s="87"/>
+      <c r="Q18" s="87"/>
+      <c r="R18" s="87"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B19" s="68">
@@ -2593,7 +2568,7 @@
         <v>106</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F19">
         <v>0.75</v>
@@ -2613,13 +2588,13 @@
       <c r="K19" s="65">
         <v>0.54212929030636825</v>
       </c>
-      <c r="L19" s="85"/>
-      <c r="M19" s="85"/>
-      <c r="N19" s="85"/>
-      <c r="O19" s="85"/>
-      <c r="P19" s="85"/>
-      <c r="Q19" s="85"/>
-      <c r="R19" s="85"/>
+      <c r="L19" s="87"/>
+      <c r="M19" s="87"/>
+      <c r="N19" s="87"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="87"/>
+      <c r="Q19" s="87"/>
+      <c r="R19" s="87"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B20" s="68">
@@ -2632,7 +2607,7 @@
         <v>106</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F20">
         <v>0.5</v>
@@ -2652,13 +2627,13 @@
       <c r="K20" s="65">
         <v>0.12759198374971206</v>
       </c>
-      <c r="L20" s="85"/>
-      <c r="M20" s="85"/>
-      <c r="N20" s="85"/>
-      <c r="O20" s="85"/>
-      <c r="P20" s="85"/>
-      <c r="Q20" s="85"/>
-      <c r="R20" s="85"/>
+      <c r="L20" s="87"/>
+      <c r="M20" s="87"/>
+      <c r="N20" s="87"/>
+      <c r="O20" s="87"/>
+      <c r="P20" s="87"/>
+      <c r="Q20" s="87"/>
+      <c r="R20" s="87"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.15">
       <c r="B21" s="68">
@@ -2671,7 +2646,7 @@
         <v>44074</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F21">
         <v>4</v>
@@ -2691,26 +2666,26 @@
       <c r="K21" s="65">
         <v>0.02</v>
       </c>
-      <c r="L21" s="86">
+      <c r="L21" s="73">
         <v>6318600</v>
       </c>
-      <c r="M21" s="86">
+      <c r="M21" s="73">
         <v>67933.333333333343</v>
       </c>
-      <c r="N21" s="86">
+      <c r="N21" s="73">
         <v>1518700</v>
       </c>
-      <c r="O21" s="86">
+      <c r="O21" s="73">
         <v>366416.66666666669</v>
       </c>
-      <c r="P21" s="86">
+      <c r="P21" s="73">
         <v>349666.66666666669</v>
       </c>
-      <c r="Q21" s="86">
+      <c r="Q21" s="73">
         <v>12333.333333333334</v>
       </c>
-      <c r="R21" s="88" t="s">
-        <v>137</v>
+      <c r="R21" s="74" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.15">
@@ -2724,7 +2699,7 @@
         <v>44074</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F22">
         <v>0.5</v>
@@ -2744,26 +2719,26 @@
       <c r="K22" s="65">
         <v>0.02</v>
       </c>
-      <c r="L22" s="86">
+      <c r="L22" s="73">
         <v>6339433.333333334</v>
       </c>
-      <c r="M22" s="86">
+      <c r="M22" s="73">
         <v>50033.333333333336</v>
       </c>
-      <c r="N22" s="86">
+      <c r="N22" s="73">
         <v>1804333.3333333335</v>
       </c>
-      <c r="O22" s="86">
+      <c r="O22" s="73">
         <v>286566.66666666669</v>
       </c>
-      <c r="P22" s="86">
+      <c r="P22" s="73">
         <v>246900</v>
       </c>
-      <c r="Q22" s="86">
+      <c r="Q22" s="73">
         <v>19933.333333333336</v>
       </c>
-      <c r="R22" s="88" t="s">
-        <v>138</v>
+      <c r="R22" s="74" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.15">
@@ -2777,7 +2752,7 @@
         <v>44074</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F23">
         <v>7.5</v>
@@ -2797,26 +2772,26 @@
       <c r="K23" s="65">
         <v>4.6726237095051619</v>
       </c>
-      <c r="L23" s="86">
+      <c r="L23" s="73">
         <v>7871466.666666667</v>
       </c>
-      <c r="M23" s="86">
+      <c r="M23" s="73">
         <v>61950</v>
       </c>
-      <c r="N23" s="86">
+      <c r="N23" s="73">
         <v>946383.33333333337</v>
       </c>
-      <c r="O23" s="86">
+      <c r="O23" s="73">
         <v>328833.33333333337</v>
       </c>
-      <c r="P23" s="86">
+      <c r="P23" s="73">
         <v>192883.33333333334</v>
       </c>
-      <c r="Q23" s="86">
+      <c r="Q23" s="73">
         <v>11566.666666666668</v>
       </c>
-      <c r="R23" s="88" t="s">
-        <v>139</v>
+      <c r="R23" s="74" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.15">
@@ -2830,7 +2805,7 @@
         <v>44074</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F24">
         <v>4</v>
@@ -2850,26 +2825,26 @@
       <c r="K24" s="65">
         <v>2.610996345854396E-2</v>
       </c>
-      <c r="L24" s="86">
+      <c r="L24" s="73">
         <v>7039000</v>
       </c>
-      <c r="M24" s="86">
+      <c r="M24" s="73">
         <v>53650</v>
       </c>
-      <c r="N24" s="86">
+      <c r="N24" s="73">
         <v>1760550</v>
       </c>
-      <c r="O24" s="86">
+      <c r="O24" s="73">
         <v>384266.66666666669</v>
       </c>
-      <c r="P24" s="86">
+      <c r="P24" s="73">
         <v>182800</v>
       </c>
-      <c r="Q24" s="86">
+      <c r="Q24" s="73">
         <v>15850</v>
       </c>
-      <c r="R24" s="88" t="s">
-        <v>140</v>
+      <c r="R24" s="74" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.15">
@@ -2883,7 +2858,7 @@
         <v>44074</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F25">
         <v>0.5</v>
@@ -2903,26 +2878,26 @@
       <c r="K25" s="65">
         <v>0.22190438297070339</v>
       </c>
-      <c r="L25" s="86">
+      <c r="L25" s="73">
         <v>6885800</v>
       </c>
-      <c r="M25" s="86">
+      <c r="M25" s="73">
         <v>51916.666666666672</v>
       </c>
-      <c r="N25" s="86">
+      <c r="N25" s="73">
         <v>1897200</v>
       </c>
-      <c r="O25" s="86">
+      <c r="O25" s="73">
         <v>354833.33333333337</v>
       </c>
-      <c r="P25" s="86">
+      <c r="P25" s="73">
         <v>147883.33333333334</v>
       </c>
-      <c r="Q25" s="86">
+      <c r="Q25" s="73">
         <v>22000</v>
       </c>
-      <c r="R25" s="88" t="s">
-        <v>141</v>
+      <c r="R25" s="74" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.15">
@@ -2936,7 +2911,7 @@
         <v>44074</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F26">
         <v>2.75</v>
@@ -2956,26 +2931,26 @@
       <c r="K26" s="65">
         <v>7.4393231838837351E-2</v>
       </c>
-      <c r="L26" s="86">
+      <c r="L26" s="73">
         <v>7084033.333333334</v>
       </c>
-      <c r="M26" s="86">
+      <c r="M26" s="73">
         <v>55450</v>
       </c>
-      <c r="N26" s="86">
+      <c r="N26" s="73">
         <v>1810100</v>
       </c>
-      <c r="O26" s="86">
+      <c r="O26" s="73">
         <v>408900</v>
       </c>
-      <c r="P26" s="86">
+      <c r="P26" s="73">
         <v>92633.333333333343</v>
       </c>
-      <c r="Q26" s="86">
+      <c r="Q26" s="73">
         <v>16633.333333333336</v>
       </c>
-      <c r="R26" s="88" t="s">
-        <v>142</v>
+      <c r="R26" s="74" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.15">
@@ -2989,7 +2964,7 @@
         <v>44074</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F27">
         <v>0.5</v>
@@ -3009,26 +2984,26 @@
       <c r="K27" s="65">
         <v>0.15194438045777228</v>
       </c>
-      <c r="L27" s="86">
+      <c r="L27" s="73">
         <v>6566066.666666667</v>
       </c>
-      <c r="M27" s="86">
+      <c r="M27" s="73">
         <v>52566.666666666672</v>
       </c>
-      <c r="N27" s="86">
+      <c r="N27" s="73">
         <v>1846866.6666666667</v>
       </c>
-      <c r="O27" s="86">
+      <c r="O27" s="73">
         <v>372216.66666666669</v>
       </c>
-      <c r="P27" s="86">
+      <c r="P27" s="73">
         <v>110083.33333333334</v>
       </c>
-      <c r="Q27" s="86">
+      <c r="Q27" s="73">
         <v>21483.333333333336</v>
       </c>
-      <c r="R27" s="88" t="s">
-        <v>143</v>
+      <c r="R27" s="74" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.15">
@@ -3042,7 +3017,7 @@
         <v>44074</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F28">
         <v>0.5</v>
@@ -3062,26 +3037,26 @@
       <c r="K28" s="65">
         <v>0.18091219399828282</v>
       </c>
-      <c r="L28" s="86">
+      <c r="L28" s="73">
         <v>6450033.333333334</v>
       </c>
-      <c r="M28" s="86">
+      <c r="M28" s="73">
         <v>50633.333333333336</v>
       </c>
-      <c r="N28" s="86">
+      <c r="N28" s="73">
         <v>1819600</v>
       </c>
-      <c r="O28" s="86">
+      <c r="O28" s="73">
         <v>367633.33333333337</v>
       </c>
-      <c r="P28" s="86">
+      <c r="P28" s="73">
         <v>109983.33333333334</v>
       </c>
-      <c r="Q28" s="86">
+      <c r="Q28" s="73">
         <v>21400</v>
       </c>
-      <c r="R28" s="88" t="s">
-        <v>144</v>
+      <c r="R28" s="74" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.15">
@@ -3095,7 +3070,7 @@
         <v>107</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F29">
         <v>4</v>
@@ -3115,26 +3090,26 @@
       <c r="K29" s="65">
         <v>1.199121934243226</v>
       </c>
-      <c r="L29" s="86">
+      <c r="L29" s="73">
         <v>5190583.333333334</v>
       </c>
-      <c r="M29" s="86">
+      <c r="M29" s="73">
         <v>74183.333333333343</v>
       </c>
-      <c r="N29" s="86">
+      <c r="N29" s="73">
         <v>331850</v>
       </c>
-      <c r="O29" s="86">
+      <c r="O29" s="73">
         <v>73533.333333333343</v>
       </c>
-      <c r="P29" s="86">
+      <c r="P29" s="73">
         <v>92866.666666666672</v>
       </c>
-      <c r="Q29" s="86">
+      <c r="Q29" s="73">
         <v>8766.6666666666679</v>
       </c>
-      <c r="R29" s="88" t="s">
-        <v>145</v>
+      <c r="R29" s="74" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.15">
@@ -3148,7 +3123,7 @@
         <v>107</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F30">
         <v>0.5</v>
@@ -3168,26 +3143,26 @@
       <c r="K30" s="65">
         <v>1.0305939882835331</v>
       </c>
-      <c r="L30" s="86">
+      <c r="L30" s="73">
         <v>5011566.666666667</v>
       </c>
-      <c r="M30" s="86">
+      <c r="M30" s="73">
         <v>42950</v>
       </c>
-      <c r="N30" s="86">
+      <c r="N30" s="73">
         <v>492283.33333333337</v>
       </c>
-      <c r="O30" s="86">
+      <c r="O30" s="73">
         <v>111100</v>
       </c>
-      <c r="P30" s="86">
+      <c r="P30" s="73">
         <v>76083.333333333343</v>
       </c>
-      <c r="Q30" s="86">
+      <c r="Q30" s="73">
         <v>12883.333333333334</v>
       </c>
-      <c r="R30" s="88" t="s">
-        <v>146</v>
+      <c r="R30" s="74" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.15">
@@ -3201,7 +3176,7 @@
         <v>107</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F31">
         <v>7.5</v>
@@ -3221,26 +3196,26 @@
       <c r="K31" s="65">
         <v>12.454265177643233</v>
       </c>
-      <c r="L31" s="86">
+      <c r="L31" s="73">
         <v>5380016.666666667</v>
       </c>
-      <c r="M31" s="86">
+      <c r="M31" s="73">
         <v>52266.666666666672</v>
       </c>
-      <c r="N31" s="86">
+      <c r="N31" s="73">
         <v>202683.33333333334</v>
       </c>
-      <c r="O31" s="86">
+      <c r="O31" s="73">
         <v>59800</v>
       </c>
-      <c r="P31" s="86">
+      <c r="P31" s="73">
         <v>146466.66666666669</v>
       </c>
-      <c r="Q31" s="86">
+      <c r="Q31" s="73">
         <v>5783.3333333333339</v>
       </c>
-      <c r="R31" s="88" t="s">
-        <v>147</v>
+      <c r="R31" s="74" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.15">
@@ -3254,7 +3229,7 @@
         <v>107</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F32">
         <v>4</v>
@@ -3274,26 +3249,26 @@
       <c r="K32" s="65">
         <v>1.3698361211623664</v>
       </c>
-      <c r="L32" s="86">
+      <c r="L32" s="73">
         <v>5294200</v>
       </c>
-      <c r="M32" s="86">
+      <c r="M32" s="73">
         <v>43966.666666666672</v>
       </c>
-      <c r="N32" s="86">
+      <c r="N32" s="73">
         <v>408700</v>
       </c>
-      <c r="O32" s="86">
+      <c r="O32" s="73">
         <v>42733.333333333336</v>
       </c>
-      <c r="P32" s="86">
+      <c r="P32" s="73">
         <v>82000</v>
       </c>
-      <c r="Q32" s="86">
+      <c r="Q32" s="73">
         <v>10166.666666666668</v>
       </c>
-      <c r="R32" s="88" t="s">
-        <v>148</v>
+      <c r="R32" s="74" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.15">
@@ -3307,7 +3282,7 @@
         <v>107</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F33">
         <v>0.5</v>
@@ -3327,26 +3302,26 @@
       <c r="K33" s="65">
         <v>2.661654672086164</v>
       </c>
-      <c r="L33" s="86">
+      <c r="L33" s="73">
         <v>4841383.333333334</v>
       </c>
-      <c r="M33" s="86">
+      <c r="M33" s="73">
         <v>34216.666666666672</v>
       </c>
-      <c r="N33" s="86">
+      <c r="N33" s="73">
         <v>294966.66666666669</v>
       </c>
-      <c r="O33" s="86">
+      <c r="O33" s="73">
         <v>132900</v>
       </c>
-      <c r="P33" s="86">
+      <c r="P33" s="73">
         <v>64583.333333333336</v>
       </c>
-      <c r="Q33" s="86">
+      <c r="Q33" s="73">
         <v>10700</v>
       </c>
-      <c r="R33" s="88" t="s">
-        <v>149</v>
+      <c r="R33" s="74" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.15">
@@ -3360,7 +3335,7 @@
         <v>107</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F34">
         <v>2.75</v>
@@ -3380,26 +3355,26 @@
       <c r="K34" s="65">
         <v>0.4611094503611759</v>
       </c>
-      <c r="L34" s="86">
+      <c r="L34" s="73">
         <v>4522966.666666667</v>
       </c>
-      <c r="M34" s="86">
+      <c r="M34" s="73">
         <v>33083.333333333336</v>
       </c>
-      <c r="N34" s="86">
+      <c r="N34" s="73">
         <v>322566.66666666669</v>
       </c>
-      <c r="O34" s="86">
+      <c r="O34" s="73">
         <v>30566.666666666668</v>
       </c>
-      <c r="P34" s="86">
+      <c r="P34" s="73">
         <v>41483.333333333336</v>
       </c>
-      <c r="Q34" s="86">
+      <c r="Q34" s="73">
         <v>7983.3333333333339</v>
       </c>
-      <c r="R34" s="88" t="s">
-        <v>150</v>
+      <c r="R34" s="74" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.15">
@@ -3413,7 +3388,7 @@
         <v>107</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F35">
         <v>0.5</v>
@@ -3433,26 +3408,26 @@
       <c r="K35" s="65">
         <v>1.0131040606079535</v>
       </c>
-      <c r="L35" s="86">
+      <c r="L35" s="73">
         <v>4902783.333333334</v>
       </c>
-      <c r="M35" s="86">
+      <c r="M35" s="73">
         <v>35333.333333333336</v>
       </c>
-      <c r="N35" s="86">
+      <c r="N35" s="73">
         <v>292400</v>
       </c>
-      <c r="O35" s="86">
+      <c r="O35" s="73">
         <v>84133.333333333343</v>
       </c>
-      <c r="P35" s="86">
+      <c r="P35" s="73">
         <v>59033.333333333336</v>
       </c>
-      <c r="Q35" s="86">
+      <c r="Q35" s="73">
         <v>9233.3333333333339</v>
       </c>
-      <c r="R35" s="88" t="s">
-        <v>151</v>
+      <c r="R35" s="74" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.15">
@@ -3466,7 +3441,7 @@
         <v>107</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F36">
         <v>0.5</v>
@@ -3486,26 +3461,26 @@
       <c r="K36" s="65">
         <v>1.835942693716565</v>
       </c>
-      <c r="L36" s="86">
+      <c r="L36" s="73">
         <v>4843850</v>
       </c>
-      <c r="M36" s="86">
+      <c r="M36" s="73">
         <v>37633.333333333336</v>
       </c>
-      <c r="N36" s="86">
+      <c r="N36" s="73">
         <v>112050</v>
       </c>
-      <c r="O36" s="86">
+      <c r="O36" s="73">
         <v>222700</v>
       </c>
-      <c r="P36" s="86">
+      <c r="P36" s="73">
         <v>88600</v>
       </c>
-      <c r="Q36" s="86">
+      <c r="Q36" s="73">
         <v>9350</v>
       </c>
-      <c r="R36" s="88" t="s">
-        <v>152</v>
+      <c r="R36" s="74" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.15">
@@ -3519,31 +3494,31 @@
         <v>108</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F37">
         <v>4</v>
       </c>
-      <c r="L37" s="86">
+      <c r="L37" s="73">
         <v>4884383.333333334</v>
       </c>
-      <c r="M37" s="86">
+      <c r="M37" s="73">
         <v>159716.66666666669</v>
       </c>
-      <c r="N37" s="86">
+      <c r="N37" s="73">
         <v>497833.33333333337</v>
       </c>
-      <c r="O37" s="86">
+      <c r="O37" s="73">
         <v>50833.333333333336</v>
       </c>
-      <c r="P37" s="86">
+      <c r="P37" s="73">
         <v>55983.333333333336</v>
       </c>
-      <c r="Q37" s="86">
+      <c r="Q37" s="73">
         <v>57900</v>
       </c>
-      <c r="R37" s="88" t="s">
-        <v>153</v>
+      <c r="R37" s="74" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.15">
@@ -3557,31 +3532,31 @@
         <v>108</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F38">
         <v>0.5</v>
       </c>
-      <c r="L38" s="86">
+      <c r="L38" s="73">
         <v>4640233.333333334</v>
       </c>
-      <c r="M38" s="86">
+      <c r="M38" s="73">
         <v>142633.33333333334</v>
       </c>
-      <c r="N38" s="86">
+      <c r="N38" s="73">
         <v>464333.33333333337</v>
       </c>
-      <c r="O38" s="86">
+      <c r="O38" s="73">
         <v>26983.333333333336</v>
       </c>
-      <c r="P38" s="86">
+      <c r="P38" s="73">
         <v>40183.333333333336</v>
       </c>
-      <c r="Q38" s="86">
+      <c r="Q38" s="73">
         <v>53950</v>
       </c>
-      <c r="R38" s="88" t="s">
-        <v>154</v>
+      <c r="R38" s="74" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.15">
@@ -3595,31 +3570,31 @@
         <v>108</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F39">
         <v>7.5</v>
       </c>
-      <c r="L39" s="86">
+      <c r="L39" s="73">
         <v>4806166.666666667</v>
       </c>
-      <c r="M39" s="86">
+      <c r="M39" s="73">
         <v>161933.33333333334</v>
       </c>
-      <c r="N39" s="86">
+      <c r="N39" s="73">
         <v>503583.33333333337</v>
       </c>
-      <c r="O39" s="86">
+      <c r="O39" s="73">
         <v>53450</v>
       </c>
-      <c r="P39" s="86">
+      <c r="P39" s="73">
         <v>57000</v>
       </c>
-      <c r="Q39" s="86">
+      <c r="Q39" s="73">
         <v>75033.333333333343</v>
       </c>
-      <c r="R39" s="88" t="s">
-        <v>155</v>
+      <c r="R39" s="74" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.15">
@@ -3633,31 +3608,31 @@
         <v>108</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F40">
         <v>4</v>
       </c>
-      <c r="L40" s="86">
+      <c r="L40" s="73">
         <v>4779266.666666667</v>
       </c>
-      <c r="M40" s="86">
+      <c r="M40" s="73">
         <v>156000</v>
       </c>
-      <c r="N40" s="86">
+      <c r="N40" s="73">
         <v>465766.66666666669</v>
       </c>
-      <c r="O40" s="86">
+      <c r="O40" s="73">
         <v>32750</v>
       </c>
-      <c r="P40" s="86">
+      <c r="P40" s="73">
         <v>49750</v>
       </c>
-      <c r="Q40" s="86">
+      <c r="Q40" s="73">
         <v>64750</v>
       </c>
-      <c r="R40" s="88" t="s">
-        <v>156</v>
+      <c r="R40" s="74" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.15">
@@ -3671,31 +3646,31 @@
         <v>108</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="F41">
         <v>0.5</v>
       </c>
-      <c r="L41" s="86">
+      <c r="L41" s="73">
         <v>4518700</v>
       </c>
-      <c r="M41" s="86">
+      <c r="M41" s="73">
         <v>150366.66666666669</v>
       </c>
-      <c r="N41" s="86">
+      <c r="N41" s="73">
         <v>426166.66666666669</v>
       </c>
-      <c r="O41" s="86">
+      <c r="O41" s="73">
         <v>28700</v>
       </c>
-      <c r="P41" s="86">
+      <c r="P41" s="73">
         <v>40833.333333333336</v>
       </c>
-      <c r="Q41" s="86">
+      <c r="Q41" s="73">
         <v>55950</v>
       </c>
-      <c r="R41" s="88" t="s">
-        <v>157</v>
+      <c r="R41" s="74" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.15">
@@ -3709,31 +3684,31 @@
         <v>108</v>
       </c>
       <c r="E42" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F42">
         <v>2.75</v>
       </c>
-      <c r="L42" s="86">
+      <c r="L42" s="73">
         <v>4391250</v>
       </c>
-      <c r="M42" s="86">
+      <c r="M42" s="73">
         <v>122633.33333333334</v>
       </c>
-      <c r="N42" s="86">
+      <c r="N42" s="73">
         <v>395633.33333333337</v>
       </c>
-      <c r="O42" s="86">
+      <c r="O42" s="73">
         <v>26750</v>
       </c>
-      <c r="P42" s="86">
+      <c r="P42" s="73">
         <v>39033.333333333336</v>
       </c>
-      <c r="Q42" s="86">
+      <c r="Q42" s="73">
         <v>48166.666666666672</v>
       </c>
-      <c r="R42" s="88" t="s">
-        <v>158</v>
+      <c r="R42" s="74" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.15">
@@ -3747,31 +3722,31 @@
         <v>108</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="F43">
         <v>0.5</v>
       </c>
-      <c r="L43" s="86">
+      <c r="L43" s="73">
         <v>4476066.666666667</v>
       </c>
-      <c r="M43" s="86">
+      <c r="M43" s="73">
         <v>128250</v>
       </c>
-      <c r="N43" s="86">
+      <c r="N43" s="73">
         <v>403866.66666666669</v>
       </c>
-      <c r="O43" s="86">
+      <c r="O43" s="73">
         <v>27533.333333333336</v>
       </c>
-      <c r="P43" s="86">
+      <c r="P43" s="73">
         <v>36900</v>
       </c>
-      <c r="Q43" s="86">
+      <c r="Q43" s="73">
         <v>53116.666666666672</v>
       </c>
-      <c r="R43" s="88" t="s">
-        <v>159</v>
+      <c r="R43" s="74" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.15">
@@ -3785,86 +3760,57 @@
         <v>108</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="F44">
         <v>0.5</v>
       </c>
-      <c r="L44" s="86">
+      <c r="L44" s="73">
         <v>4626883.333333334</v>
       </c>
-      <c r="M44" s="86">
+      <c r="M44" s="73">
         <v>134816.66666666669</v>
       </c>
-      <c r="N44" s="86">
+      <c r="N44" s="73">
         <v>443466.66666666669</v>
       </c>
-      <c r="O44" s="86">
+      <c r="O44" s="73">
         <v>25800</v>
       </c>
-      <c r="P44" s="86">
+      <c r="P44" s="73">
         <v>36550</v>
       </c>
-      <c r="Q44" s="86">
+      <c r="Q44" s="73">
         <v>52116.666666666672</v>
       </c>
-      <c r="R44" s="88" t="s">
-        <v>160</v>
+      <c r="R44" s="74" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.15">
-      <c r="B48" s="67" t="s">
-        <v>99</v>
-      </c>
+      <c r="B48" s="67"/>
       <c r="C48" s="67"/>
-      <c r="D48" s="20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B49" s="67" t="s">
-        <v>110</v>
-      </c>
+      <c r="D48" s="20"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B49" s="67"/>
       <c r="C49" s="67"/>
-      <c r="D49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B50" s="67" t="s">
-        <v>111</v>
-      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B50" s="67"/>
       <c r="C50" s="67"/>
-      <c r="D50">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B51" s="67" t="s">
-        <v>112</v>
-      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B51" s="67"/>
       <c r="C51" s="67"/>
-      <c r="D51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B52" s="67" t="s">
-        <v>113</v>
-      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B52" s="67"/>
       <c r="C52" s="67"/>
-      <c r="D52">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B53" s="67" t="s">
-        <v>114</v>
-      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.15">
+      <c r="B53" s="67"/>
       <c r="C53" s="67"/>
-      <c r="D53">
-        <v>5</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -3946,7 +3892,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="71" t="s">
+      <c r="A13" s="75" t="s">
         <v>93</v>
       </c>
       <c r="B13" s="33" t="s">
@@ -3961,15 +3907,15 @@
       <c r="E13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="73" t="s">
+      <c r="G13" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="73" t="s">
+      <c r="H13" s="77" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="72"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="34" t="s">
         <v>16</v>
       </c>
@@ -3982,8 +3928,8 @@
       <c r="E14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="21">
@@ -4104,11 +4050,11 @@
         <f>'Chlorophyll a'!H13</f>
         <v>3.4499999999999997</v>
       </c>
-      <c r="J18" s="74" t="s">
+      <c r="J18" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
+      <c r="K18" s="78"/>
+      <c r="L18" s="78"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A19" s="21">
@@ -4138,9 +4084,9 @@
         <f>'Chlorophyll a'!H14</f>
         <v>2.58</v>
       </c>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
+      <c r="J19" s="78"/>
+      <c r="K19" s="78"/>
+      <c r="L19" s="78"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A20" s="21">
@@ -4170,9 +4116,9 @@
         <f>'Chlorophyll a'!H15</f>
         <v>2.415</v>
       </c>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A21" s="21">
@@ -4202,9 +4148,9 @@
         <f>'Chlorophyll a'!H16</f>
         <v>2.7600000000000002</v>
       </c>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
+      <c r="J21" s="78"/>
+      <c r="K21" s="78"/>
+      <c r="L21" s="78"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A22" s="21">
@@ -7522,13 +7468,13 @@
       <c r="E34" s="35">
         <v>0.50490230980252548</v>
       </c>
-      <c r="G34" s="78" t="s">
+      <c r="G34" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
+      <c r="H34" s="83"/>
+      <c r="I34" s="83"/>
+      <c r="J34" s="83"/>
+      <c r="K34" s="83"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A35" s="21" t="s">
@@ -7546,11 +7492,11 @@
       <c r="E35" s="35">
         <v>5.717590517873222</v>
       </c>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="79"/>
-      <c r="J35" s="79"/>
-      <c r="K35" s="79"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A36" s="21" t="s">
@@ -7607,12 +7553,12 @@
       <c r="E38" s="40">
         <v>101.0733209546669</v>
       </c>
-      <c r="G38" s="75" t="s">
+      <c r="G38" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="77"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="81"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A39" s="32" t="s">
@@ -7948,20 +7894,20 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="78" t="s">
+      <c r="A56" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="79"/>
-      <c r="C56" s="79"/>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="83"/>
+      <c r="D56" s="83"/>
+      <c r="E56" s="83"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="79"/>
-      <c r="B57" s="79"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="79"/>
-      <c r="E57" s="79"/>
+      <c r="A57" s="83"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="83"/>
+      <c r="D57" s="83"/>
+      <c r="E57" s="83"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A58" s="51"/>
@@ -7972,12 +7918,12 @@
     </row>
     <row r="59" spans="1:5" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="75" t="s">
+      <c r="A60" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="76"/>
-      <c r="C60" s="76"/>
-      <c r="D60" s="77"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="81"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A61" s="23"/>
@@ -8241,11 +8187,11 @@
         <f t="shared" si="2"/>
         <v>0.26750000000000002</v>
       </c>
-      <c r="J11" s="74" t="s">
+      <c r="J11" s="78" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="74"/>
-      <c r="L11" s="74"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="78"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A12" s="50">
@@ -8275,9 +8221,9 @@
         <f t="shared" si="2"/>
         <v>5.5949999999999998</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="74"/>
-      <c r="L12" s="74"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="78"/>
+      <c r="L12" s="78"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A13" s="50">
@@ -8307,9 +8253,9 @@
         <f t="shared" si="2"/>
         <v>3.4499999999999997</v>
       </c>
-      <c r="J13" s="74"/>
-      <c r="K13" s="74"/>
-      <c r="L13" s="74"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="78"/>
+      <c r="L13" s="78"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A14" s="50">
@@ -8339,9 +8285,9 @@
         <f>F14/G14*1000</f>
         <v>2.58</v>
       </c>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
+      <c r="J14" s="78"/>
+      <c r="K14" s="78"/>
+      <c r="L14" s="78"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A15" s="50">
@@ -8405,13 +8351,13 @@
       <c r="A17" s="50">
         <v>1.8</v>
       </c>
-      <c r="B17" s="80" t="s">
+      <c r="B17" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="81"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="81"/>
-      <c r="F17" s="82"/>
+      <c r="C17" s="85"/>
+      <c r="D17" s="85"/>
+      <c r="E17" s="85"/>
+      <c r="F17" s="86"/>
       <c r="G17" s="60"/>
       <c r="H17" s="59"/>
     </row>

</xml_diff>

<commit_message>
Create oyster and clam visualizations
</commit_message>
<xml_diff>
--- a/data/raw/2024-02-28_water-samples.xlsx
+++ b/data/raw/2024-02-28_water-samples.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lysbethkoster/Documents/Universiteit/University of Hawai'i/MSc Thesis/Thesis/RQ2/nomilo-fishpond-analysis/data/raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hawaii0-my.sharepoint.com/personal/alemarie_hawaii_edu/Documents/Desktop/nomilo-fishpond-analysis/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6285CBA7-10C2-2349-B276-B15624E1557C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6285CBA7-10C2-2349-B276-B15624E1557C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA2C67D7-FA6C-4075-B7D0-0391861EDB75}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2295" yWindow="2070" windowWidth="12300" windowHeight="11235" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Overview" sheetId="14" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1182,6 +1182,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1217,11 +1221,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1683,28 +1682,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="10.83203125" style="68"/>
-    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+    <col min="2" max="3" width="10.875" style="68"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
     <col min="7" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="18.5" customWidth="1"/>
-    <col min="10" max="10" width="22.83203125" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
-    <col min="12" max="12" width="16.1640625" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="18.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="28.25" customWidth="1"/>
+    <col min="12" max="12" width="16.125" customWidth="1"/>
+    <col min="13" max="13" width="18.875" customWidth="1"/>
+    <col min="14" max="14" width="17.625" customWidth="1"/>
+    <col min="15" max="15" width="18.375" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
     <col min="17" max="17" width="19.5" customWidth="1"/>
-    <col min="18" max="18" width="14.83203125" customWidth="1"/>
+    <col min="18" max="18" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="55" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" s="55" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>112</v>
       </c>
@@ -1760,7 +1759,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B2" s="68">
         <v>1.1000000000000001</v>
       </c>
@@ -1813,7 +1812,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B3" s="68">
         <v>1.2</v>
       </c>
@@ -1866,7 +1865,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B4" s="68">
         <v>1.3</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B5" s="68">
         <v>1.4</v>
       </c>
@@ -1972,7 +1971,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B6" s="68">
         <v>1.5</v>
       </c>
@@ -2025,7 +2024,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B7" s="68">
         <v>1.6</v>
       </c>
@@ -2078,7 +2077,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B8" s="68">
         <v>1.7</v>
       </c>
@@ -2131,7 +2130,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="68">
         <v>1.8</v>
       </c>
@@ -2159,29 +2158,29 @@
       <c r="K9" s="65">
         <v>10.237966201076372</v>
       </c>
-      <c r="L9" s="88">
+      <c r="L9" s="75">
         <v>1522316.6666666667</v>
       </c>
-      <c r="M9" s="88">
+      <c r="M9" s="75">
         <v>403766.66666666669</v>
       </c>
-      <c r="N9" s="88">
+      <c r="N9" s="75">
         <v>65216.666666666672</v>
       </c>
-      <c r="O9" s="88">
+      <c r="O9" s="75">
         <v>6916.666666666667</v>
       </c>
-      <c r="P9" s="88">
+      <c r="P9" s="75">
         <v>93783.333333333343</v>
       </c>
-      <c r="Q9" s="88">
+      <c r="Q9" s="75">
         <v>616.66666666666674</v>
       </c>
-      <c r="R9" s="89" t="s">
+      <c r="R9" s="76" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B10" s="68">
         <v>1.9</v>
       </c>
@@ -2234,7 +2233,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B11" s="69">
         <v>1.1000000000000001</v>
       </c>
@@ -2284,7 +2283,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B12" s="68">
         <v>2.1</v>
       </c>
@@ -2315,15 +2314,8 @@
       <c r="K12" s="65">
         <v>0.17575021464620025</v>
       </c>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
-      <c r="N12" s="87"/>
-      <c r="O12" s="87"/>
-      <c r="P12" s="87"/>
-      <c r="Q12" s="87"/>
-      <c r="R12" s="87"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B13" s="68">
         <v>2.2000000000000002</v>
       </c>
@@ -2354,15 +2346,8 @@
       <c r="K13" s="65">
         <v>0.50490230980252548</v>
       </c>
-      <c r="L13" s="87"/>
-      <c r="M13" s="87"/>
-      <c r="N13" s="87"/>
-      <c r="O13" s="87"/>
-      <c r="P13" s="87"/>
-      <c r="Q13" s="87"/>
-      <c r="R13" s="87"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B14" s="68">
         <v>2.2999999999999998</v>
       </c>
@@ -2393,15 +2378,8 @@
       <c r="K14" s="65">
         <v>5.717590517873222</v>
       </c>
-      <c r="L14" s="87"/>
-      <c r="M14" s="87"/>
-      <c r="N14" s="87"/>
-      <c r="O14" s="87"/>
-      <c r="P14" s="87"/>
-      <c r="Q14" s="87"/>
-      <c r="R14" s="87"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B15" s="68">
         <v>2.4</v>
       </c>
@@ -2432,15 +2410,8 @@
       <c r="K15" s="65">
         <v>0.1225544217838834</v>
       </c>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B16" s="68">
         <v>2.5</v>
       </c>
@@ -2471,15 +2442,8 @@
       <c r="K16" s="65">
         <v>0.40063032689045719</v>
       </c>
-      <c r="L16" s="87"/>
-      <c r="M16" s="87"/>
-      <c r="N16" s="87"/>
-      <c r="O16" s="87"/>
-      <c r="P16" s="87"/>
-      <c r="Q16" s="87"/>
-      <c r="R16" s="87"/>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="68">
         <v>2.6</v>
       </c>
@@ -2510,15 +2474,8 @@
       <c r="K17" s="65">
         <v>0.22172219546415931</v>
       </c>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="87"/>
-      <c r="Q17" s="87"/>
-      <c r="R17" s="87"/>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="68">
         <v>2.7</v>
       </c>
@@ -2549,15 +2506,8 @@
       <c r="K18" s="65">
         <v>0.46476032919397736</v>
       </c>
-      <c r="L18" s="87"/>
-      <c r="M18" s="87"/>
-      <c r="N18" s="87"/>
-      <c r="O18" s="87"/>
-      <c r="P18" s="87"/>
-      <c r="Q18" s="87"/>
-      <c r="R18" s="87"/>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="68">
         <v>2.8</v>
       </c>
@@ -2588,15 +2538,8 @@
       <c r="K19" s="65">
         <v>0.54212929030636825</v>
       </c>
-      <c r="L19" s="87"/>
-      <c r="M19" s="87"/>
-      <c r="N19" s="87"/>
-      <c r="O19" s="87"/>
-      <c r="P19" s="87"/>
-      <c r="Q19" s="87"/>
-      <c r="R19" s="87"/>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="68">
         <v>2.9</v>
       </c>
@@ -2627,15 +2570,8 @@
       <c r="K20" s="65">
         <v>0.12759198374971206</v>
       </c>
-      <c r="L20" s="87"/>
-      <c r="M20" s="87"/>
-      <c r="N20" s="87"/>
-      <c r="O20" s="87"/>
-      <c r="P20" s="87"/>
-      <c r="Q20" s="87"/>
-      <c r="R20" s="87"/>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.15">
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="68">
         <v>3.1</v>
       </c>
@@ -2688,7 +2624,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="68">
         <v>3.2</v>
       </c>
@@ -2741,7 +2677,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="68">
         <v>3.3</v>
       </c>
@@ -2794,7 +2730,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="68">
         <v>3.4</v>
       </c>
@@ -2847,7 +2783,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="68">
         <v>3.5</v>
       </c>
@@ -2900,7 +2836,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" s="68">
         <v>3.6</v>
       </c>
@@ -2953,7 +2889,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" s="68">
         <v>3.7</v>
       </c>
@@ -3006,7 +2942,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="68">
         <v>3.8</v>
       </c>
@@ -3059,7 +2995,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="68">
         <v>4.0999999999999996</v>
       </c>
@@ -3112,7 +3048,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" s="68">
         <v>4.2</v>
       </c>
@@ -3165,7 +3101,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" s="68">
         <v>4.3</v>
       </c>
@@ -3218,7 +3154,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="32" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="68">
         <v>4.4000000000000004</v>
       </c>
@@ -3271,7 +3207,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B33" s="68">
         <v>4.5</v>
       </c>
@@ -3324,7 +3260,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B34" s="68">
         <v>4.5999999999999996</v>
       </c>
@@ -3377,7 +3313,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="35" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B35" s="68">
         <v>4.7</v>
       </c>
@@ -3430,7 +3366,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="36" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B36" s="68">
         <v>4.8</v>
       </c>
@@ -3483,7 +3419,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B37" s="68">
         <v>5.0999999999999996</v>
       </c>
@@ -3521,7 +3457,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="38" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B38" s="68">
         <v>5.2</v>
       </c>
@@ -3559,7 +3495,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B39" s="68">
         <v>5.3</v>
       </c>
@@ -3597,7 +3533,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B40" s="68">
         <v>5.4</v>
       </c>
@@ -3635,7 +3571,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="41" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B41" s="68">
         <v>5.5</v>
       </c>
@@ -3673,7 +3609,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="42" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B42" s="68">
         <v>5.6</v>
       </c>
@@ -3711,7 +3647,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B43" s="68">
         <v>5.7</v>
       </c>
@@ -3749,7 +3685,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="44" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B44" s="68">
         <v>5.8</v>
       </c>
@@ -3787,28 +3723,28 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B48" s="67"/>
       <c r="C48" s="67"/>
       <c r="D48" s="20"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B49" s="67"/>
       <c r="C49" s="67"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B50" s="67"/>
       <c r="C50" s="67"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B51" s="67"/>
       <c r="C51" s="67"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B52" s="67"/>
       <c r="C52" s="67"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B53" s="67"/>
       <c r="C53" s="67"/>
     </row>
@@ -3826,53 +3762,53 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="20.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D1" s="19" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D9" s="64" t="s">
         <v>8</v>
       </c>
@@ -3880,10 +3816,10 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D10" s="64"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D11" s="64" t="s">
         <v>9</v>
       </c>
@@ -3891,8 +3827,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="75" t="s">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="77" t="s">
         <v>93</v>
       </c>
       <c r="B13" s="33" t="s">
@@ -3907,15 +3843,15 @@
       <c r="E13" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="H13" s="77" t="s">
+      <c r="H13" s="79" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A14" s="76"/>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="78"/>
       <c r="B14" s="34" t="s">
         <v>16</v>
       </c>
@@ -3928,10 +3864,10 @@
       <c r="E14" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="77"/>
-      <c r="H14" s="77"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="21">
         <v>1.1000000000000001</v>
       </c>
@@ -3961,7 +3897,7 @@
         <v>2.0399999999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="21">
         <v>1.2</v>
       </c>
@@ -3991,7 +3927,7 @@
         <v>0.26750000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="21">
         <v>1.3</v>
       </c>
@@ -4021,7 +3957,7 @@
         <v>5.5949999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:12" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="21">
         <v>1.4</v>
       </c>
@@ -4050,13 +3986,13 @@
         <f>'Chlorophyll a'!H13</f>
         <v>3.4499999999999997</v>
       </c>
-      <c r="J18" s="78" t="s">
+      <c r="J18" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="K18" s="78"/>
-      <c r="L18" s="78"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K18" s="80"/>
+      <c r="L18" s="80"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
         <v>1.5</v>
       </c>
@@ -4084,11 +4020,11 @@
         <f>'Chlorophyll a'!H14</f>
         <v>2.58</v>
       </c>
-      <c r="J19" s="78"/>
-      <c r="K19" s="78"/>
-      <c r="L19" s="78"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+      <c r="L19" s="80"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>1.6</v>
       </c>
@@ -4116,11 +4052,11 @@
         <f>'Chlorophyll a'!H15</f>
         <v>2.415</v>
       </c>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+      <c r="L20" s="80"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>1.7</v>
       </c>
@@ -4148,11 +4084,11 @@
         <f>'Chlorophyll a'!H16</f>
         <v>2.7600000000000002</v>
       </c>
-      <c r="J21" s="78"/>
-      <c r="K21" s="78"/>
-      <c r="L21" s="78"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+      <c r="L21" s="80"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>1.8</v>
       </c>
@@ -4180,7 +4116,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>1.9</v>
       </c>
@@ -4209,7 +4145,7 @@
         <v>1.7399999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="22">
         <v>1.1000000000000001</v>
       </c>
@@ -4230,7 +4166,7 @@
         <v>1.1989759805666658</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>2.1</v>
       </c>
@@ -4259,7 +4195,7 @@
         <v>5.7692307692307692</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
         <v>2.2000000000000002</v>
       </c>
@@ -4288,7 +4224,7 @@
         <v>4.8239999999999998</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>2.2999999999999998</v>
       </c>
@@ -4317,7 +4253,7 @@
         <v>5.2714285714285722</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>2.4</v>
       </c>
@@ -4346,7 +4282,7 @@
         <v>4.1307692307692312</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>2.5</v>
       </c>
@@ -4375,7 +4311,7 @@
         <v>3.6749999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
         <v>2.6</v>
       </c>
@@ -4404,7 +4340,7 @@
         <v>4.2599999999999989</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="21">
         <v>2.7</v>
       </c>
@@ -4433,7 +4369,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="21">
         <v>2.8</v>
       </c>
@@ -4462,7 +4398,7 @@
         <v>2.3307692307692309</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="21">
         <v>2.9</v>
       </c>
@@ -4491,7 +4427,7 @@
         <v>1.4850000000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="21">
         <v>3.1</v>
       </c>
@@ -4520,7 +4456,7 @@
         <v>2.5500000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
         <v>3.2</v>
       </c>
@@ -4549,7 +4485,7 @@
         <v>3.2700000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="21">
         <v>3.3</v>
       </c>
@@ -4578,7 +4514,7 @@
         <v>1.575</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="21">
         <v>3.4</v>
       </c>
@@ -4607,7 +4543,7 @@
         <v>5.8950000000000005</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="21">
         <v>3.5</v>
       </c>
@@ -4636,7 +4572,7 @@
         <v>1.4654999999999998</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="21">
         <v>3.6</v>
       </c>
@@ -4665,7 +4601,7 @@
         <v>2.4599999999999995</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="21">
         <v>3.7</v>
       </c>
@@ -4694,7 +4630,7 @@
         <v>3.0600000000000005</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="21">
         <v>3.8</v>
       </c>
@@ -4723,7 +4659,7 @@
         <v>3.8222222222222224</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="21">
         <v>4.0999999999999996</v>
       </c>
@@ -4752,7 +4688,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="21">
         <v>4.2</v>
       </c>
@@ -4781,7 +4717,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="21">
         <v>4.3</v>
       </c>
@@ -4810,7 +4746,7 @@
         <v>5.6142857142857148</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="21">
         <v>4.4000000000000004</v>
       </c>
@@ -4839,7 +4775,7 @@
         <v>5.1150000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="21">
         <v>4.5</v>
       </c>
@@ -4868,7 +4804,7 @@
         <v>0.87450000000000017</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="21">
         <v>4.5999999999999996</v>
       </c>
@@ -4897,7 +4833,7 @@
         <v>0.42250000000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="21">
         <v>4.7</v>
       </c>
@@ -4926,7 +4862,7 @@
         <v>0.11299999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="21">
         <v>4.8</v>
       </c>
@@ -4978,18 +4914,18 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>10</v>
       </c>
@@ -5005,7 +4941,7 @@
       <c r="J1" s="11"/>
       <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="13"/>
       <c r="B2" s="14" t="s">
         <v>23</v>
@@ -5033,7 +4969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="13"/>
       <c r="B3" s="17" t="s">
         <v>16</v>
@@ -5061,7 +4997,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="36">
         <f>'Nutrient Channels DATA'!A23</f>
         <v>396</v>
@@ -5103,7 +5039,7 @@
         <v>0.55166376981550902</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="36" t="str">
         <f>'Nutrient Channels DATA'!A24</f>
         <v>367</v>
@@ -5145,7 +5081,7 @@
         <v>7.5972190228886141E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="36" t="str">
         <f>'Nutrient Channels DATA'!A25</f>
         <v>398</v>
@@ -5187,7 +5123,7 @@
         <v>3.2685653257386971</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="36" t="str">
         <f>'Nutrient Channels DATA'!A26</f>
         <v>399</v>
@@ -5229,7 +5165,7 @@
         <v>1.0934286851087889</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="str">
         <f>'Nutrient Channels DATA'!A27</f>
         <v>400</v>
@@ -5271,7 +5207,7 @@
         <v>0.11344208740812095</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="36" t="str">
         <f>'Nutrient Channels DATA'!A28</f>
         <v>401</v>
@@ -5313,7 +5249,7 @@
         <v>0.32313990744037024</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="str">
         <f>'Nutrient Channels DATA'!A29</f>
         <v>402</v>
@@ -5355,7 +5291,7 @@
         <v>0.47799928800284797</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="36" t="str">
         <f>'Nutrient Channels DATA'!A30</f>
         <v>403</v>
@@ -5397,7 +5333,7 @@
         <v>10.237966201076372</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="str">
         <f>'Nutrient Channels DATA'!A31</f>
         <v>404</v>
@@ -5439,7 +5375,7 @@
         <v>0.29314368064819812</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="36" t="str">
         <f>'Nutrient Channels DATA'!A32</f>
         <v>405</v>
@@ -5481,7 +5417,7 @@
         <v>1.1989759805666658</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="36" t="str">
         <f>'Nutrient Channels DATA'!A33</f>
         <v>406</v>
@@ -5523,7 +5459,7 @@
         <v>0.17575021464620025</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="36" t="str">
         <f>'Nutrient Channels DATA'!A34</f>
         <v>407</v>
@@ -5565,7 +5501,7 @@
         <v>0.50490230980252548</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="36" t="str">
         <f>'Nutrient Channels DATA'!A35</f>
         <v>408</v>
@@ -5607,7 +5543,7 @@
         <v>5.717590517873222</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="36" t="str">
         <f>'Nutrient Channels DATA'!A36</f>
         <v>409</v>
@@ -5649,7 +5585,7 @@
         <v>0.1225544217838834</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="36" t="str">
         <f>'Nutrient Channels DATA'!A40</f>
         <v>410</v>
@@ -5691,7 +5627,7 @@
         <v>0.40063032689045719</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="36" t="str">
         <f>'Nutrient Channels DATA'!A41</f>
         <v>411</v>
@@ -5733,7 +5669,7 @@
         <v>0.22172219546415931</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="36" t="str">
         <f>'Nutrient Channels DATA'!A42</f>
         <v>412</v>
@@ -5775,7 +5711,7 @@
         <v>0.46476032919397736</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="36" t="str">
         <f>'Nutrient Channels DATA'!A43</f>
         <v>413</v>
@@ -5817,7 +5753,7 @@
         <v>0.54212929030636825</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="36" t="str">
         <f>'Nutrient Channels DATA'!A44</f>
         <v>414</v>
@@ -5859,7 +5795,7 @@
         <v>0.12759198374971206</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="36" t="str">
         <f>'Nutrient Channels DATA'!A45</f>
         <v>415</v>
@@ -5901,7 +5837,7 @@
         <v>&lt;0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="36" t="str">
         <f>'Nutrient Channels DATA'!A46</f>
         <v>416</v>
@@ -5943,7 +5879,7 @@
         <v>&lt;0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="36" t="str">
         <f>'Nutrient Channels DATA'!A47</f>
         <v>417</v>
@@ -5985,7 +5921,7 @@
         <v>4.6726237095051619</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="36" t="str">
         <f>'Nutrient Channels DATA'!A48</f>
         <v>418</v>
@@ -6027,7 +5963,7 @@
         <v>2.610996345854396E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="36" t="str">
         <f>'Nutrient Channels DATA'!A49</f>
         <v>419</v>
@@ -6069,7 +6005,7 @@
         <v>0.22190438297070339</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="36" t="str">
         <f>'Nutrient Channels DATA'!A50</f>
         <v>420</v>
@@ -6111,7 +6047,7 @@
         <v>7.4393231838837351E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="36" t="str">
         <f>'Nutrient Channels DATA'!A51</f>
         <v>421</v>
@@ -6153,7 +6089,7 @@
         <v>0.15194438045777228</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="36">
         <f>'Nutrient Channels DATA'!A52</f>
         <v>422</v>
@@ -6195,7 +6131,7 @@
         <v>0.18091219399828282</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="36">
         <f>'Nutrient Channels DATA'!G23</f>
         <v>1</v>
@@ -6237,7 +6173,7 @@
         <v>1.199121934243226</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="36" t="str">
         <f>'Nutrient Channels DATA'!G24</f>
         <v>2</v>
@@ -6279,7 +6215,7 @@
         <v>1.0305939882835331</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="36" t="str">
         <f>'Nutrient Channels DATA'!G25</f>
         <v>3</v>
@@ -6321,7 +6257,7 @@
         <v>12.454265177643233</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="36" t="str">
         <f>'Nutrient Channels DATA'!G26</f>
         <v>4</v>
@@ -6363,7 +6299,7 @@
         <v>1.3698361211623664</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="36" t="str">
         <f>'Nutrient Channels DATA'!G27</f>
         <v>5</v>
@@ -6405,7 +6341,7 @@
         <v>2.661654672086164</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="36" t="str">
         <f>'Nutrient Channels DATA'!G28</f>
         <v>6</v>
@@ -6447,7 +6383,7 @@
         <v>0.4611094503611759</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="36" t="str">
         <f>'Nutrient Channels DATA'!G29</f>
         <v>7</v>
@@ -6489,7 +6425,7 @@
         <v>1.0131040606079535</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="36">
         <f>'Nutrient Channels DATA'!G30</f>
         <v>8</v>
@@ -6547,17 +6483,17 @@
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.33203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -6571,7 +6507,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -6585,7 +6521,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -6599,7 +6535,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -6613,8 +6549,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="2">
         <v>3</v>
@@ -6642,7 +6578,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
@@ -6674,7 +6610,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -6706,7 +6642,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -6738,7 +6674,7 @@
         <v>-11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
@@ -6770,7 +6706,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>19</v>
       </c>
@@ -6802,7 +6738,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>20</v>
       </c>
@@ -6834,7 +6770,7 @@
         <v>0.99874879070103861</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>21</v>
       </c>
@@ -6844,7 +6780,7 @@
       </c>
       <c r="H14" s="19"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="29" t="s">
         <v>22</v>
       </c>
@@ -6876,7 +6812,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="29" t="s">
         <v>22</v>
       </c>
@@ -6908,7 +6844,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="29" t="s">
         <v>22</v>
       </c>
@@ -6940,7 +6876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="29" t="s">
         <v>22</v>
       </c>
@@ -6972,7 +6908,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="29" t="s">
         <v>22</v>
       </c>
@@ -7004,7 +6940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>30</v>
       </c>
@@ -7036,7 +6972,7 @@
         <v>5.9431352758321232E-5</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>28</v>
       </c>
@@ -7068,7 +7004,7 @@
         <v>99.067928947882095</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>28</v>
       </c>
@@ -7100,7 +7036,7 @@
         <v>97.667382393129017</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="42">
         <v>396</v>
       </c>
@@ -7132,7 +7068,7 @@
         <v>1.199121934243226</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
         <v>52</v>
       </c>
@@ -7164,7 +7100,7 @@
         <v>1.0305939882835331</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
         <v>53</v>
       </c>
@@ -7196,7 +7132,7 @@
         <v>12.454265177643233</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
         <v>54</v>
       </c>
@@ -7228,7 +7164,7 @@
         <v>1.3698361211623664</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
         <v>55</v>
       </c>
@@ -7260,7 +7196,7 @@
         <v>2.661654672086164</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
         <v>56</v>
       </c>
@@ -7292,7 +7228,7 @@
         <v>0.4611094503611759</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
         <v>57</v>
       </c>
@@ -7324,7 +7260,7 @@
         <v>1.0131040606079535</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
         <v>58</v>
       </c>
@@ -7356,7 +7292,7 @@
         <v>1.835942693716565</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="21" t="s">
         <v>59</v>
       </c>
@@ -7388,7 +7324,7 @@
         <v>7.4956832895341496E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
         <v>60</v>
       </c>
@@ -7420,7 +7356,7 @@
         <v>102.833333333333</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
         <v>61</v>
       </c>
@@ -7452,7 +7388,7 @@
         <v>103.372549019608</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
         <v>62</v>
       </c>
@@ -7468,15 +7404,15 @@
       <c r="E34" s="35">
         <v>0.50490230980252548</v>
       </c>
-      <c r="G34" s="82" t="s">
+      <c r="G34" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="H34" s="83"/>
-      <c r="I34" s="83"/>
-      <c r="J34" s="83"/>
-      <c r="K34" s="83"/>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H34" s="85"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="85"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
         <v>63</v>
       </c>
@@ -7492,13 +7428,13 @@
       <c r="E35" s="35">
         <v>5.717590517873222</v>
       </c>
-      <c r="G35" s="83"/>
-      <c r="H35" s="83"/>
-      <c r="I35" s="83"/>
-      <c r="J35" s="83"/>
-      <c r="K35" s="83"/>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="G35" s="85"/>
+      <c r="H35" s="85"/>
+      <c r="I35" s="85"/>
+      <c r="J35" s="85"/>
+      <c r="K35" s="85"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
         <v>64</v>
       </c>
@@ -7520,7 +7456,7 @@
       <c r="J36" s="51"/>
       <c r="K36" s="51"/>
     </row>
-    <row r="37" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30" t="s">
         <v>30</v>
       </c>
@@ -7537,7 +7473,7 @@
         <v>8.9879169895085084E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
         <v>28</v>
       </c>
@@ -7553,14 +7489,14 @@
       <c r="E38" s="40">
         <v>101.0733209546669</v>
       </c>
-      <c r="G38" s="79" t="s">
+      <c r="G38" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H38" s="80"/>
-      <c r="I38" s="80"/>
-      <c r="J38" s="81"/>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="83"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>28</v>
       </c>
@@ -7587,7 +7523,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="42" t="s">
         <v>65</v>
       </c>
@@ -7614,7 +7550,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
         <v>66</v>
       </c>
@@ -7643,7 +7579,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
         <v>67</v>
       </c>
@@ -7672,7 +7608,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
         <v>68</v>
       </c>
@@ -7689,7 +7625,7 @@
         <v>0.54212929030636825</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
         <v>69</v>
       </c>
@@ -7706,7 +7642,7 @@
         <v>0.12759198374971206</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
         <v>70</v>
       </c>
@@ -7723,7 +7659,7 @@
         <v>6.0729168848028259E-5</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
         <v>71</v>
       </c>
@@ -7740,7 +7676,7 @@
         <v>2.7328125981613688E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="21" t="s">
         <v>72</v>
       </c>
@@ -7757,7 +7693,7 @@
         <v>4.6726237095051619</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
         <v>73</v>
       </c>
@@ -7774,7 +7710,7 @@
         <v>2.610996345854396E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
         <v>74</v>
       </c>
@@ -7791,7 +7727,7 @@
         <v>0.22190438297070339</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
         <v>75</v>
       </c>
@@ -7808,7 +7744,7 @@
         <v>7.4393231838837351E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
         <v>76</v>
       </c>
@@ -7825,7 +7761,7 @@
         <v>0.15194438045777228</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="21">
         <v>422</v>
       </c>
@@ -7842,7 +7778,7 @@
         <v>0.18091219399828282</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="30" t="s">
         <v>30</v>
       </c>
@@ -7859,7 +7795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
         <v>28</v>
       </c>
@@ -7876,7 +7812,7 @@
         <v>102.49082921969112</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
         <v>28</v>
       </c>
@@ -7893,39 +7829,39 @@
         <v>103.2878945699923</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A56" s="82" t="s">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="B56" s="83"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="83"/>
-      <c r="E56" s="83"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A57" s="83"/>
-      <c r="B57" s="83"/>
-      <c r="C57" s="83"/>
-      <c r="D57" s="83"/>
-      <c r="E57" s="83"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B56" s="85"/>
+      <c r="C56" s="85"/>
+      <c r="D56" s="85"/>
+      <c r="E56" s="85"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="85"/>
+      <c r="B57" s="85"/>
+      <c r="C57" s="85"/>
+      <c r="D57" s="85"/>
+      <c r="E57" s="85"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="51"/>
       <c r="B58" s="51"/>
       <c r="C58" s="51"/>
       <c r="D58" s="51"/>
       <c r="E58" s="51"/>
     </row>
-    <row r="59" spans="1:5" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A60" s="79" t="s">
+    <row r="59" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="80"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="81"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="B60" s="82"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="83"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="23"/>
       <c r="B61" s="21" t="s">
         <v>23</v>
@@ -7937,7 +7873,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="23"/>
       <c r="B62" s="21" t="s">
         <v>31</v>
@@ -7949,7 +7885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="23" t="s">
         <v>32</v>
       </c>
@@ -7963,7 +7899,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="14" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
         <v>0</v>
       </c>
@@ -7999,16 +7935,16 @@
       <selection activeCell="B17" sqref="B17:F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="256" width="8.83203125" customWidth="1"/>
+    <col min="1" max="1" width="8.875" customWidth="1"/>
+    <col min="2" max="2" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.875" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="6" max="256" width="8.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="55" t="s">
         <v>90</v>
       </c>
@@ -8022,7 +7958,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="55" t="s">
         <v>78</v>
       </c>
@@ -8036,7 +7972,7 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="55" t="s">
         <v>79</v>
       </c>
@@ -8050,7 +7986,7 @@
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -8060,7 +7996,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="55" t="s">
         <v>80</v>
       </c>
@@ -8072,7 +8008,7 @@
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
         <v>81</v>
       </c>
@@ -8084,7 +8020,7 @@
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -8094,7 +8030,7 @@
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="20"/>
       <c r="C8" s="20"/>
@@ -8104,7 +8040,7 @@
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:12" ht="42" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:12" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A9" s="56" t="s">
         <v>82</v>
       </c>
@@ -8130,7 +8066,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="50">
         <v>1.1000000000000001</v>
       </c>
@@ -8159,7 +8095,7 @@
         <v>2.0399999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="50">
         <v>1.2</v>
       </c>
@@ -8187,13 +8123,13 @@
         <f t="shared" si="2"/>
         <v>0.26750000000000002</v>
       </c>
-      <c r="J11" s="78" t="s">
+      <c r="J11" s="80" t="s">
         <v>94</v>
       </c>
-      <c r="K11" s="78"/>
-      <c r="L11" s="78"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="K11" s="80"/>
+      <c r="L11" s="80"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="50">
         <v>1.3</v>
       </c>
@@ -8221,11 +8157,11 @@
         <f t="shared" si="2"/>
         <v>5.5949999999999998</v>
       </c>
-      <c r="J12" s="78"/>
-      <c r="K12" s="78"/>
-      <c r="L12" s="78"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J12" s="80"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="80"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="50">
         <v>1.4</v>
       </c>
@@ -8253,11 +8189,11 @@
         <f t="shared" si="2"/>
         <v>3.4499999999999997</v>
       </c>
-      <c r="J13" s="78"/>
-      <c r="K13" s="78"/>
-      <c r="L13" s="78"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J13" s="80"/>
+      <c r="K13" s="80"/>
+      <c r="L13" s="80"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="50">
         <v>1.5</v>
       </c>
@@ -8285,11 +8221,11 @@
         <f>F14/G14*1000</f>
         <v>2.58</v>
       </c>
-      <c r="J14" s="78"/>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="J14" s="80"/>
+      <c r="K14" s="80"/>
+      <c r="L14" s="80"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="50">
         <v>1.6</v>
       </c>
@@ -8318,7 +8254,7 @@
         <v>2.415</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="50">
         <v>1.7</v>
       </c>
@@ -8347,21 +8283,21 @@
         <v>2.7600000000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="50">
         <v>1.8</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="86"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="87"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="88"/>
       <c r="G17" s="60"/>
       <c r="H17" s="59"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="50">
         <v>1.9</v>
       </c>
@@ -8390,7 +8326,7 @@
         <v>1.7399999999999998</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="50">
         <v>2.1</v>
       </c>
@@ -8419,7 +8355,7 @@
         <v>5.7692307692307692</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="50">
         <v>2.2000000000000002</v>
       </c>
@@ -8448,7 +8384,7 @@
         <v>4.8239999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="50">
         <v>2.2999999999999998</v>
       </c>
@@ -8477,7 +8413,7 @@
         <v>5.2714285714285722</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="50">
         <v>2.4</v>
       </c>
@@ -8506,7 +8442,7 @@
         <v>4.1307692307692312</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="50">
         <v>2.5</v>
       </c>
@@ -8535,7 +8471,7 @@
         <v>3.6749999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="50">
         <v>2.6</v>
       </c>
@@ -8564,7 +8500,7 @@
         <v>4.2599999999999989</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="50">
         <v>2.7</v>
       </c>
@@ -8593,7 +8529,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="50">
         <v>2.8</v>
       </c>
@@ -8622,7 +8558,7 @@
         <v>2.3307692307692309</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="50">
         <v>2.9</v>
       </c>
@@ -8651,7 +8587,7 @@
         <v>1.4850000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="50">
         <v>3.1</v>
       </c>
@@ -8680,7 +8616,7 @@
         <v>2.5500000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="50">
         <v>3.2</v>
       </c>
@@ -8709,7 +8645,7 @@
         <v>3.2700000000000005</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="50">
         <v>3.3</v>
       </c>
@@ -8738,7 +8674,7 @@
         <v>1.575</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="50">
         <v>3.4</v>
       </c>
@@ -8767,7 +8703,7 @@
         <v>5.8950000000000005</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="50">
         <v>3.5</v>
       </c>
@@ -8796,7 +8732,7 @@
         <v>1.4654999999999998</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="50">
         <v>3.6</v>
       </c>
@@ -8825,7 +8761,7 @@
         <v>2.4599999999999995</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="50">
         <v>3.7</v>
       </c>
@@ -8854,7 +8790,7 @@
         <v>3.0600000000000005</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="50">
         <v>3.8</v>
       </c>
@@ -8883,7 +8819,7 @@
         <v>3.8222222222222224</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="50">
         <v>4.0999999999999996</v>
       </c>
@@ -8912,7 +8848,7 @@
         <v>8.25</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="50">
         <v>4.2</v>
       </c>
@@ -8941,7 +8877,7 @@
         <v>1.89</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="50">
         <v>4.3</v>
       </c>
@@ -8970,7 +8906,7 @@
         <v>5.6142857142857148</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="50">
         <v>4.4000000000000004</v>
       </c>
@@ -8999,7 +8935,7 @@
         <v>5.1150000000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="50">
         <v>4.5</v>
       </c>
@@ -9028,7 +8964,7 @@
         <v>0.87450000000000017</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="50">
         <v>4.5999999999999996</v>
       </c>
@@ -9057,7 +8993,7 @@
         <v>0.42250000000000004</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="50">
         <v>4.7</v>
       </c>
@@ -9086,7 +9022,7 @@
         <v>0.11299999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="50">
         <v>4.8</v>
       </c>

</xml_diff>